<commit_message>
Updated PCB with new header
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Lightsaber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D965B4-FE25-FA4F-B3F9-C488D34E4FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F977CA63-6153-2B4A-9A78-16355E465E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17000" xr2:uid="{96C7B9D5-BF93-5C45-B977-7D9E9A39640F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>ERJ-6ENF2001V</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/vishay-beyschlag-draloric-bc-components/MCU08050D5002BP100/8125783</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0015910100/614775</t>
   </si>
 </sst>
 </file>
@@ -603,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357E0829-7B57-F84A-BFEE-FBF8F03996E1}">
-  <dimension ref="A2:D22"/>
+  <dimension ref="A2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,6 +908,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <v>15910100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>